<commit_message>
correção do saldo de empregos
</commit_message>
<xml_diff>
--- a/salvo_excel/saldo_por_mes_ma.xlsx
+++ b/salvo_excel/saldo_por_mes_ma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOVO\Documents\TCC\novocaged\salvo_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D69AF-D854-4C0A-9B49-7CFBDE6450A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA7523A-E645-4889-8AA5-98FDF3C17D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="1596" windowWidth="13872" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>competenciamov</t>
   </si>
   <si>
-    <t>saldo_ajuste</t>
-  </si>
-  <si>
     <t>admitidos_ajuste</t>
   </si>
   <si>
@@ -215,6 +212,15 @@
   </si>
   <si>
     <t>2024/12</t>
+  </si>
+  <si>
+    <t>Total do MA</t>
+  </si>
+  <si>
+    <t>Complexo Portuário do MA</t>
+  </si>
+  <si>
+    <t>saldo_ajuste_MA</t>
   </si>
 </sst>
 </file>
@@ -306,18 +312,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>saldo_ajuste</c:v>
+                  <c:v>Total do MA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent4"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -327,7 +333,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:f>Sheet1!$H$2:$H$61</c:f>
               <c:strCache>
                 <c:ptCount val="60"/>
                 <c:pt idx="0">
@@ -515,7 +521,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$61</c:f>
+              <c:f>Sheet1!$I$2:$I$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -704,7 +710,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BBB2-4951-B368-7E64E2988409}"/>
+              <c16:uniqueId val="{00000000-3EC5-4DD5-A9F2-63E50F0140A8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -716,12 +722,439 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="50"/>
-        <c:axId val="1915695951"/>
-        <c:axId val="1918801503"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1908925727"/>
+        <c:axId val="1825127295"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Complexo Portuário do MA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$H$2:$H$61</c:f>
+              <c:strCache>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2020/01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020/02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2020/03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2020/04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2020/05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2020/06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2020/07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2020/08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020/09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2020/10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2020/11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2020/12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2021/01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2021/02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2021/03</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2021/04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2021/05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2021/06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2021/07</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2021/08</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2021/09</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021/10</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2021/11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2021/12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2022/01</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2022/02</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2022/03</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2022/04</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2022/05</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2022/06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2022/07</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2022/08</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2022/09</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2022/10</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2022/11</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2022/12</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2023/01</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2023/02</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2023/03</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2023/04</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2023/05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2023/06</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2023/07</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2023/08</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2023/09</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2023/10</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2023/11</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2023/12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2024/01</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2024/02</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2024/03</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2024/04</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2024/05</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2024/06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2024/07</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2024/08</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2024/09</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2024/10</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2024/11</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2024/12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-140</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-56</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-48</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-42</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3EC5-4DD5-A9F2-63E50F0140A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1908928607"/>
+        <c:axId val="1825122335"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="1915695951"/>
+        <c:axId val="1908925727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +1178,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -761,7 +1194,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1918801503"/>
+        <c:crossAx val="1825127295"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -769,12 +1202,61 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1918801503"/>
+        <c:axId val="1825127295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Saldo total do Maranhão</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -803,10 +1285,121 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1915695951"/>
+        <c:crossAx val="1908925727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="1825122335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Saldo do Complexo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-BR" baseline="0"/>
+                  <a:t> Portuário do MA</a:t>
+                </a:r>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1908928607"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1908928607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1825122335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -815,6 +1408,34 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -828,7 +1449,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:noFill/>
@@ -1407,23 +2028,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>239890</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>168487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>514209</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>160867</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067392A1-B992-1BC1-952E-C5A9D50A6845}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{239A2FD5-EB52-CE9D-CCB8-22340EE347B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1731,37 +2352,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="H42" zoomScale="108" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>202001</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>488</v>
@@ -1772,13 +2405,22 @@
       <c r="E2">
         <v>13278</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>488</v>
+      </c>
+      <c r="J2">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>202002</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>2331</v>
@@ -1789,13 +2431,22 @@
       <c r="E3">
         <v>11625</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>2331</v>
+      </c>
+      <c r="J3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>202003</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>-1880</v>
@@ -1806,13 +2457,22 @@
       <c r="E4">
         <v>14786</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>-1880</v>
+      </c>
+      <c r="J4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>202004</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>-6926</v>
@@ -1823,13 +2483,22 @@
       <c r="E5">
         <v>15024</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>-6926</v>
+      </c>
+      <c r="J5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>202005</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>-1736</v>
@@ -1840,13 +2509,22 @@
       <c r="E6">
         <v>12101</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>-1736</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>202006</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>3262</v>
@@ -1857,13 +2535,22 @@
       <c r="E7">
         <v>10105</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>3262</v>
+      </c>
+      <c r="J7">
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>202007</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>5251</v>
@@ -1874,13 +2561,22 @@
       <c r="E8">
         <v>10605</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>5251</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>202008</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>5908</v>
@@ -1891,13 +2587,22 @@
       <c r="E9">
         <v>11504</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9">
+        <v>5908</v>
+      </c>
+      <c r="J9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>202009</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>5424</v>
@@ -1908,13 +2613,22 @@
       <c r="E10">
         <v>11894</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>5424</v>
+      </c>
+      <c r="J10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>202010</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>5827</v>
@@ -1925,13 +2639,22 @@
       <c r="E11">
         <v>12820</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11">
+        <v>5827</v>
+      </c>
+      <c r="J11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>202011</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>3925</v>
@@ -1942,13 +2665,22 @@
       <c r="E12">
         <v>12960</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <v>3925</v>
+      </c>
+      <c r="J12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>202012</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>-4413</v>
@@ -1959,13 +2691,22 @@
       <c r="E13">
         <v>16829</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>-4413</v>
+      </c>
+      <c r="J13">
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>202101</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>151</v>
@@ -1976,13 +2717,22 @@
       <c r="E14">
         <v>18371</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>151</v>
+      </c>
+      <c r="J14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>202102</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>4036</v>
@@ -1993,13 +2743,22 @@
       <c r="E15">
         <v>14962</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>4036</v>
+      </c>
+      <c r="J15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>202103</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>4004</v>
@@ -2010,13 +2769,22 @@
       <c r="E16">
         <v>14917</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>4004</v>
+      </c>
+      <c r="J16">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>202104</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>3018</v>
@@ -2027,13 +2795,22 @@
       <c r="E17">
         <v>14473</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>3018</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>202105</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>4154</v>
@@ -2044,13 +2821,22 @@
       <c r="E18">
         <v>13935</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>4154</v>
+      </c>
+      <c r="J18">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>202106</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>7537</v>
@@ -2061,13 +2847,22 @@
       <c r="E19">
         <v>13323</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19">
+        <v>7537</v>
+      </c>
+      <c r="J19">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>202107</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>5704</v>
@@ -2078,13 +2873,22 @@
       <c r="E20">
         <v>15095</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>5704</v>
+      </c>
+      <c r="J20">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>202108</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>5435</v>
@@ -2095,13 +2899,22 @@
       <c r="E21">
         <v>15158</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21">
+        <v>5435</v>
+      </c>
+      <c r="J21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>202109</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>3879</v>
@@ -2112,13 +2925,22 @@
       <c r="E22">
         <v>15971</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22">
+        <v>3879</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>202110</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>5846</v>
@@ -2129,13 +2951,22 @@
       <c r="E23">
         <v>14811</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23">
+        <v>5846</v>
+      </c>
+      <c r="J23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>202111</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>2797</v>
@@ -2146,13 +2977,22 @@
       <c r="E24">
         <v>16086</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24">
+        <v>2797</v>
+      </c>
+      <c r="J24">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>202112</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>-1624</v>
@@ -2163,13 +3003,22 @@
       <c r="E25">
         <v>17635</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25">
+        <v>-1624</v>
+      </c>
+      <c r="J25">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>202201</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>970</v>
@@ -2180,13 +3029,22 @@
       <c r="E26">
         <v>18469</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26">
+        <v>970</v>
+      </c>
+      <c r="J26">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>202202</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>4515</v>
@@ -2197,13 +3055,22 @@
       <c r="E27">
         <v>17149</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27">
+        <v>4515</v>
+      </c>
+      <c r="J27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>202203</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>1451</v>
@@ -2214,13 +3081,22 @@
       <c r="E28">
         <v>18659</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28">
+        <v>1451</v>
+      </c>
+      <c r="J28">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>202204</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>3605</v>
@@ -2231,13 +3107,22 @@
       <c r="E29">
         <v>17240</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29">
+        <v>3605</v>
+      </c>
+      <c r="J29">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>202205</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>5074</v>
@@ -2248,13 +3133,22 @@
       <c r="E30">
         <v>18072</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30">
+        <v>5074</v>
+      </c>
+      <c r="J30">
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>202206</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>6737</v>
@@ -2265,13 +3159,22 @@
       <c r="E31">
         <v>17283</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31">
+        <v>6737</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>202207</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>5757</v>
@@ -2282,13 +3185,22 @@
       <c r="E32">
         <v>18213</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32">
+        <v>5757</v>
+      </c>
+      <c r="J32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>202208</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>5555</v>
@@ -2299,13 +3211,22 @@
       <c r="E33">
         <v>19931</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33">
+        <v>5555</v>
+      </c>
+      <c r="J33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>202209</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>7057</v>
@@ -2316,13 +3237,22 @@
       <c r="E34">
         <v>17057</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I34">
+        <v>7057</v>
+      </c>
+      <c r="J34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>202210</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>3154</v>
@@ -2333,13 +3263,22 @@
       <c r="E35">
         <v>17549</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35">
+        <v>3154</v>
+      </c>
+      <c r="J35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>202211</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36">
         <v>1728</v>
@@ -2350,13 +3289,22 @@
       <c r="E36">
         <v>18546</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36">
+        <v>1728</v>
+      </c>
+      <c r="J36">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>202212</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37">
         <v>-5300</v>
@@ -2367,13 +3315,22 @@
       <c r="E37">
         <v>20764</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <v>-5300</v>
+      </c>
+      <c r="J37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>202301</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>1466</v>
@@ -2384,13 +3341,22 @@
       <c r="E38">
         <v>19123</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38">
+        <v>1466</v>
+      </c>
+      <c r="J38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>202302</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>954</v>
@@ -2401,13 +3367,22 @@
       <c r="E39">
         <v>17656</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I39">
+        <v>954</v>
+      </c>
+      <c r="J39">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>202303</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>2669</v>
@@ -2418,13 +3393,22 @@
       <c r="E40">
         <v>19445</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40">
+        <v>2669</v>
+      </c>
+      <c r="J40">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>202304</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>1969</v>
@@ -2435,13 +3419,22 @@
       <c r="E41">
         <v>17094</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I41">
+        <v>1969</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>202305</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42">
         <v>2377</v>
@@ -2452,13 +3445,22 @@
       <c r="E42">
         <v>18344</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42">
+        <v>2377</v>
+      </c>
+      <c r="J42">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>202306</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43">
         <v>4665</v>
@@ -2469,13 +3471,22 @@
       <c r="E43">
         <v>19277</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43">
+        <v>4665</v>
+      </c>
+      <c r="J43">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>202307</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>2718</v>
@@ -2486,13 +3497,22 @@
       <c r="E44">
         <v>18713</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I44">
+        <v>2718</v>
+      </c>
+      <c r="J44">
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>202308</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45">
         <v>2475</v>
@@ -2503,13 +3523,22 @@
       <c r="E45">
         <v>20855</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>47</v>
+      </c>
+      <c r="I45">
+        <v>2475</v>
+      </c>
+      <c r="J45">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>202309</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46">
         <v>2933</v>
@@ -2520,13 +3549,22 @@
       <c r="E46">
         <v>19087</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46">
+        <v>2933</v>
+      </c>
+      <c r="J46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>202310</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <v>2303</v>
@@ -2537,13 +3575,22 @@
       <c r="E47">
         <v>19086</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>49</v>
+      </c>
+      <c r="I47">
+        <v>2303</v>
+      </c>
+      <c r="J47">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>202311</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>1358</v>
@@ -2554,13 +3601,22 @@
       <c r="E48">
         <v>18831</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>50</v>
+      </c>
+      <c r="I48">
+        <v>1358</v>
+      </c>
+      <c r="J48">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>202312</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>-4024</v>
@@ -2571,13 +3627,22 @@
       <c r="E49">
         <v>19055</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>51</v>
+      </c>
+      <c r="I49">
+        <v>-4024</v>
+      </c>
+      <c r="J49">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>202401</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50">
         <v>-762</v>
@@ -2588,13 +3653,22 @@
       <c r="E50">
         <v>21579</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50">
+        <v>-762</v>
+      </c>
+      <c r="J50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>202402</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51">
         <v>-2721</v>
@@ -2605,13 +3679,22 @@
       <c r="E51">
         <v>22524</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51">
+        <v>-2721</v>
+      </c>
+      <c r="J51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>202403</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52">
         <v>2776</v>
@@ -2622,13 +3705,22 @@
       <c r="E52">
         <v>19803</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52">
+        <v>2776</v>
+      </c>
+      <c r="J52">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>202404</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>2831</v>
@@ -2639,13 +3731,22 @@
       <c r="E53">
         <v>19762</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53">
+        <v>2831</v>
+      </c>
+      <c r="J53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>202405</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54">
         <v>2881</v>
@@ -2656,13 +3757,22 @@
       <c r="E54">
         <v>20455</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>56</v>
+      </c>
+      <c r="I54">
+        <v>2881</v>
+      </c>
+      <c r="J54">
+        <v>-48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>202406</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55">
         <v>6192</v>
@@ -2673,13 +3783,22 @@
       <c r="E55">
         <v>19071</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I55">
+        <v>6192</v>
+      </c>
+      <c r="J55">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>202407</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56">
         <v>2938</v>
@@ -2690,13 +3809,22 @@
       <c r="E56">
         <v>20661</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>58</v>
+      </c>
+      <c r="I56">
+        <v>2938</v>
+      </c>
+      <c r="J56">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>202408</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57">
         <v>2697</v>
@@ -2707,13 +3835,22 @@
       <c r="E57">
         <v>21051</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>59</v>
+      </c>
+      <c r="I57">
+        <v>2697</v>
+      </c>
+      <c r="J57">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>202409</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>4481</v>
@@ -2724,13 +3861,22 @@
       <c r="E58">
         <v>18803</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>60</v>
+      </c>
+      <c r="I58">
+        <v>4481</v>
+      </c>
+      <c r="J58">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>202410</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59">
         <v>560</v>
@@ -2741,13 +3887,22 @@
       <c r="E59">
         <v>21760</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59">
+        <v>560</v>
+      </c>
+      <c r="J59">
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>202411</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60">
         <v>1457</v>
@@ -2758,13 +3913,22 @@
       <c r="E60">
         <v>20078</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H60" t="s">
+        <v>62</v>
+      </c>
+      <c r="I60">
+        <v>1457</v>
+      </c>
+      <c r="J60">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>202412</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61">
         <v>-7003</v>
@@ -2774,6 +3938,15 @@
       </c>
       <c r="E61">
         <v>22803</v>
+      </c>
+      <c r="H61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I61">
+        <v>-7003</v>
+      </c>
+      <c r="J61">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>